<commit_message>
Fix critical attendance state issue by resolving client-side state inversion and server-side sorting. Implemented robust error handling for type casting in attendance records. Enhanced UI responsiveness with listener-based updates across multiple tabs. Added new features for forced attendance with immediate UI feedback and detailed logging for debugging.
</commit_message>
<xml_diff>
--- a/server/reports/attendance_report.xlsx
+++ b/server/reports/attendance_report.xlsx
@@ -11,103 +11,163 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="50">
+  <si>
+    <t>Nome Dipendente</t>
+  </si>
+  <si>
+    <t>Cantiere</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Data e Ora</t>
+  </si>
+  <si>
+    <t>Dispositivo</t>
+  </si>
+  <si>
+    <t>Latitudine</t>
+  </si>
+  <si>
+    <t>Longitudine</t>
+  </si>
+  <si>
+    <t>Google Maps</t>
+  </si>
   <si>
     <t>ID Dipendente</t>
   </si>
   <si>
-    <t>Nome Dipendente</t>
-  </si>
-  <si>
-    <t>Cantiere</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Data e Ora</t>
-  </si>
-  <si>
-    <t>Dispositivo</t>
-  </si>
-  <si>
-    <t>Latitudine</t>
-  </si>
-  <si>
-    <t>Longitudine</t>
-  </si>
-  <si>
-    <t>tom</t>
-  </si>
-  <si>
-    <t>knmkn</t>
+    <t>Tommaso</t>
+  </si>
+  <si>
+    <t>Lecce</t>
   </si>
   <si>
     <t>Uscita</t>
   </si>
   <si>
-    <t>13/10/2025, 21:00:58</t>
+    <t>14/10/2025, 19:11:14</t>
+  </si>
+  <si>
+    <t>Forced by admin: Admin</t>
+  </si>
+  <si>
+    <t>N/D</t>
+  </si>
+  <si>
+    <t>Ingresso</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:09:14</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:08:39</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:08:24</t>
+  </si>
+  <si>
+    <t>android - SP1A.210812.016</t>
+  </si>
+  <si>
+    <t>40.352793</t>
+  </si>
+  <si>
+    <t>18.160146</t>
+  </si>
+  <si>
+    <t>Apri in Maps</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:03:39</t>
   </si>
   <si>
     <t>windows - "Windows 10 Pro" 10.0 (Build 26100)</t>
   </si>
   <si>
-    <t>N/D</t>
-  </si>
-  <si>
-    <t>Ingresso</t>
-  </si>
-  <si>
-    <t>13/10/2025, 21:00:44</t>
-  </si>
-  <si>
-    <t>lecce</t>
-  </si>
-  <si>
-    <t>13/10/2025, 20:22:14</t>
-  </si>
-  <si>
-    <t>android - SP1A.210812.016</t>
-  </si>
-  <si>
-    <t>40.352814</t>
-  </si>
-  <si>
-    <t>18.160023</t>
-  </si>
-  <si>
-    <t>13/10/2025, 20:15:16</t>
-  </si>
-  <si>
-    <t>40.352813</t>
-  </si>
-  <si>
-    <t>18.160025</t>
-  </si>
-  <si>
-    <t>13/10/2025, 19:45:58</t>
-  </si>
-  <si>
-    <t>40.352819</t>
-  </si>
-  <si>
-    <t>18.160047</t>
-  </si>
-  <si>
-    <t>13/10/2025, 19:44:41</t>
-  </si>
-  <si>
-    <t>40.352812</t>
-  </si>
-  <si>
-    <t>18.160059</t>
+    <t>40.351500</t>
+  </si>
+  <si>
+    <t>18.175000</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:03:11</t>
+  </si>
+  <si>
+    <t>Forced by admin: Admin | Note: INGRESSO FORZATO</t>
+  </si>
+  <si>
+    <t>14/10/2025, 19:02:22</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:55:57</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:53:49</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:44:06</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:40:10</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:18:36</t>
+  </si>
+  <si>
+    <t>Oria</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:16:30</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:04:58</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:59:14</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:56:23</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:52:10</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:51:21</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:45:53</t>
+  </si>
+  <si>
+    <t>Forced by admin: Admin | Note: forzata prova</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:40:54</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:40:27</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:38:06</t>
+  </si>
+  <si>
+    <t>Forced by admin: Admin | Note: timbratura out forzata</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:18:17</t>
+  </si>
+  <si>
+    <t>14/10/2025, 18:17:41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -126,6 +186,10 @@
     <font>
       <b/>
       <color rgb="FF00B050"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0563C1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,6 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,19 +572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="8" width="15" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,165 +610,719 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>5</v>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>29</v>
+      <c r="H9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:I1"/>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
+    <hyperlink ref="H10" r:id="rId4"/>
+    <hyperlink ref="H11" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="H15" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Implement employee deletion flow with forced OUT timestamp and automatic attendance management
</commit_message>
<xml_diff>
--- a/server/reports/attendance_report.xlsx
+++ b/server/reports/attendance_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Nome Dipendente</t>
   </si>
@@ -40,7 +40,7 @@
     <t>ID Dipendente</t>
   </si>
   <si>
-    <t>Tommaso</t>
+    <t>k</t>
   </si>
   <si>
     <t>Lecce</t>
@@ -49,52 +49,28 @@
     <t>Uscita</t>
   </si>
   <si>
-    <t>14/10/2025, 20:09:29</t>
+    <t>14/10/2025, 21:05:14</t>
+  </si>
+  <si>
+    <t>Forzato da ATommaso | Note: Timbratura OUT automatica prima dell'eliminazione</t>
+  </si>
+  <si>
+    <t>N/D</t>
+  </si>
+  <si>
+    <t>Ingresso</t>
+  </si>
+  <si>
+    <t>14/10/2025, 21:05:11</t>
   </si>
   <si>
     <t>Forzato da ATommaso</t>
   </si>
   <si>
-    <t>N/D</t>
-  </si>
-  <si>
-    <t>Ingresso</t>
-  </si>
-  <si>
-    <t>14/10/2025, 20:08:42</t>
-  </si>
-  <si>
-    <t>Forzato da ATommaso | Note: ????</t>
-  </si>
-  <si>
-    <t>14/10/2025, 20:07:53</t>
-  </si>
-  <si>
-    <t>Forzato da Admin | Note: cccccccccccc</t>
-  </si>
-  <si>
-    <t>14/10/2025, 20:04:49</t>
-  </si>
-  <si>
-    <t>Forced by admin: Admin | Note: BAAAABBBBBB</t>
-  </si>
-  <si>
-    <t>14/10/2025, 20:02:10</t>
-  </si>
-  <si>
-    <t>Forced by admin: Admin | Note: timbratura FORZATAAAAAAAA</t>
-  </si>
-  <si>
-    <t>14/10/2025, 19:51:47</t>
-  </si>
-  <si>
-    <t>Forced by admin: Admin</t>
-  </si>
-  <si>
-    <t>14/10/2025, 19:38:47</t>
-  </si>
-  <si>
-    <t>14/10/2025, 19:37:41</t>
+    <t>14/10/2025, 21:04:54</t>
+  </si>
+  <si>
+    <t>14/10/2025, 21:04:34</t>
   </si>
   <si>
     <t>windows - "Windows 10 Pro" 10.0 (Build 26100)</t>
@@ -518,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
@@ -586,7 +562,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -615,7 +591,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -632,7 +608,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>14</v>
@@ -644,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -658,144 +634,28 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>